<commit_message>
Update Category and Get Food from Criteria
</commit_message>
<xml_diff>
--- a/AHP Sản phẩm Món chính.xlsx
+++ b/AHP Sản phẩm Món chính.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\OneDrive - hcmunre.edu.vn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhokk\Desktop\HoTroRaQuyetDinh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6999B43B-0C09-4DFA-A505-21F0E9B51F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164E3906-E2BB-433B-B3A1-AC39D3184B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{738D0DCC-DACC-4475-BFCE-0371B9E87382}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{738D0DCC-DACC-4475-BFCE-0371B9E87382}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="30">
   <si>
     <t>Calo</t>
   </si>
@@ -124,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +238,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -277,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -300,12 +334,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -393,10 +438,38 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
     <cellStyle name="Bình thường 2" xfId="1" xr:uid="{6427199B-9DB9-407B-BD68-8167036689A6}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -411,24 +484,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -724,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8420C6-B896-437C-BDF8-F9FED97D9E93}">
-  <dimension ref="C8:AH287"/>
+  <dimension ref="C8:AH312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T218" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AE241" sqref="AE241"/>
+    <sheetView topLeftCell="J92" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V116" sqref="V116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2914,19 +2971,19 @@
       <c r="Z101" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AA101" s="28" t="s">
+      <c r="AA101" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AB101" s="28" t="s">
+      <c r="AB101" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="AC101" s="28" t="s">
+      <c r="AC101" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AD101" s="28" t="s">
+      <c r="AD101" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="AE101" s="28" t="s">
+      <c r="AE101" s="36" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2949,19 +3006,19 @@
       <c r="Z102" s="12">
         <v>2</v>
       </c>
-      <c r="AA102" s="12">
+      <c r="AA102" s="8">
         <v>2</v>
       </c>
-      <c r="AB102" s="12">
+      <c r="AB102" s="8">
         <v>0.25</v>
       </c>
-      <c r="AC102" s="12">
+      <c r="AC102" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AD102" s="12">
+      <c r="AD102" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AE102" s="12">
+      <c r="AE102" s="8">
         <v>1.5</v>
       </c>
     </row>
@@ -2984,19 +3041,19 @@
       <c r="Z103" s="12">
         <v>3</v>
       </c>
-      <c r="AA103" s="12">
+      <c r="AA103" s="8">
         <v>3</v>
       </c>
-      <c r="AB103" s="12">
+      <c r="AB103" s="8">
         <v>0.5</v>
       </c>
-      <c r="AC103" s="12">
+      <c r="AC103" s="8">
         <v>0.5</v>
       </c>
-      <c r="AD103" s="12">
+      <c r="AD103" s="8">
         <v>1.5</v>
       </c>
-      <c r="AE103" s="12">
+      <c r="AE103" s="8">
         <v>3</v>
       </c>
     </row>
@@ -3019,19 +3076,19 @@
       <c r="Z104" s="12">
         <v>3</v>
       </c>
-      <c r="AA104" s="12">
+      <c r="AA104" s="8">
         <v>3</v>
       </c>
-      <c r="AB104" s="12">
+      <c r="AB104" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC104" s="12">
+      <c r="AC104" s="8">
         <v>0.5</v>
       </c>
-      <c r="AD104" s="12">
+      <c r="AD104" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="AE104" s="12">
+      <c r="AE104" s="8">
         <v>3</v>
       </c>
     </row>
@@ -3054,19 +3111,19 @@
       <c r="Z105" s="12">
         <v>2</v>
       </c>
-      <c r="AA105" s="12">
+      <c r="AA105" s="8">
         <v>2</v>
       </c>
-      <c r="AB105" s="12">
+      <c r="AB105" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC105" s="12">
+      <c r="AC105" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AD105" s="12">
+      <c r="AD105" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AE105" s="12">
+      <c r="AE105" s="8">
         <v>0.5</v>
       </c>
     </row>
@@ -3089,238 +3146,238 @@
       <c r="Z106" s="12">
         <v>1</v>
       </c>
-      <c r="AA106" s="12">
+      <c r="AA106" s="8">
         <v>1.5</v>
       </c>
-      <c r="AB106" s="12">
+      <c r="AB106" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC106" s="12">
+      <c r="AC106" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AD106" s="12">
+      <c r="AD106" s="8">
         <v>0.5</v>
       </c>
-      <c r="AE106" s="12">
+      <c r="AE106" s="8">
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="107" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="U107" s="27" t="s">
+      <c r="U107" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="V107" s="12">
+      <c r="V107" s="8">
         <v>0.5</v>
       </c>
-      <c r="W107" s="12">
+      <c r="W107" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="X107" s="12">
+      <c r="X107" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Y107" s="12">
+      <c r="Y107" s="8">
         <v>0.5</v>
       </c>
-      <c r="Z107" s="12">
+      <c r="Z107" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="AA107" s="12">
+      <c r="AA107" s="8">
         <v>1</v>
       </c>
-      <c r="AB107" s="12">
+      <c r="AB107" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC107" s="12">
+      <c r="AC107" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AD107" s="12">
+      <c r="AD107" s="8">
         <v>0.5</v>
       </c>
-      <c r="AE107" s="12">
+      <c r="AE107" s="8">
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="108" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="U108" s="27" t="s">
+      <c r="U108" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="V108" s="12">
+      <c r="V108" s="8">
         <v>4</v>
       </c>
-      <c r="W108" s="12">
+      <c r="W108" s="8">
         <v>2</v>
       </c>
-      <c r="X108" s="12">
+      <c r="X108" s="8">
         <v>3</v>
       </c>
-      <c r="Y108" s="12">
+      <c r="Y108" s="8">
         <v>3</v>
       </c>
-      <c r="Z108" s="12">
+      <c r="Z108" s="8">
         <v>3</v>
       </c>
-      <c r="AA108" s="12">
+      <c r="AA108" s="8">
         <v>3</v>
       </c>
-      <c r="AB108" s="12">
+      <c r="AB108" s="8">
         <v>1</v>
       </c>
-      <c r="AC108" s="12">
+      <c r="AC108" s="8">
         <v>2</v>
       </c>
-      <c r="AD108" s="12">
+      <c r="AD108" s="8">
         <v>3</v>
       </c>
-      <c r="AE108" s="12">
+      <c r="AE108" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="109" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="U109" s="27" t="s">
+      <c r="U109" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="V109" s="12">
+      <c r="V109" s="8">
         <v>3</v>
       </c>
-      <c r="W109" s="12">
+      <c r="W109" s="8">
         <v>2</v>
       </c>
-      <c r="X109" s="12">
+      <c r="X109" s="8">
         <v>2</v>
       </c>
-      <c r="Y109" s="12">
+      <c r="Y109" s="8">
         <v>3</v>
       </c>
-      <c r="Z109" s="12">
+      <c r="Z109" s="8">
         <v>3</v>
       </c>
-      <c r="AA109" s="12">
+      <c r="AA109" s="8">
         <v>3</v>
       </c>
-      <c r="AB109" s="12">
+      <c r="AB109" s="8">
         <v>0.5</v>
       </c>
-      <c r="AC109" s="12">
+      <c r="AC109" s="8">
         <v>1</v>
       </c>
-      <c r="AD109" s="12">
+      <c r="AD109" s="8">
         <v>2</v>
       </c>
-      <c r="AE109" s="12">
+      <c r="AE109" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="110" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="U110" s="27" t="s">
+      <c r="U110" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="V110" s="12">
+      <c r="V110" s="8">
         <v>3</v>
       </c>
-      <c r="W110" s="12">
+      <c r="W110" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="X110" s="12">
+      <c r="X110" s="8">
         <v>1.5</v>
       </c>
-      <c r="Y110" s="12">
+      <c r="Y110" s="8">
         <v>3</v>
       </c>
-      <c r="Z110" s="12">
+      <c r="Z110" s="8">
         <v>2</v>
       </c>
-      <c r="AA110" s="12">
+      <c r="AA110" s="8">
         <v>2</v>
       </c>
-      <c r="AB110" s="12">
+      <c r="AB110" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC110" s="12">
+      <c r="AC110" s="8">
         <v>0.5</v>
       </c>
-      <c r="AD110" s="12">
+      <c r="AD110" s="8">
         <v>1</v>
       </c>
-      <c r="AE110" s="12">
+      <c r="AE110" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="111" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="U111" s="27" t="s">
+      <c r="U111" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="V111" s="12">
+      <c r="V111" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="W111" s="12">
+      <c r="W111" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="X111" s="12">
+      <c r="X111" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Y111" s="12">
+      <c r="Y111" s="8">
         <v>2</v>
       </c>
-      <c r="Z111" s="12">
+      <c r="Z111" s="8">
         <v>1.5</v>
       </c>
-      <c r="AA111" s="12">
+      <c r="AA111" s="8">
         <v>1.5</v>
       </c>
-      <c r="AB111" s="12">
+      <c r="AB111" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC111" s="12">
+      <c r="AC111" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AD111" s="12">
+      <c r="AD111" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AE111" s="12">
+      <c r="AE111" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="21:34" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="U112" s="17" t="s">
+      <c r="U112" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="V112" s="16">
+      <c r="V112" s="35">
         <f>SUM(V102:V111)</f>
         <v>18.333333333333336</v>
       </c>
-      <c r="W112" s="16">
+      <c r="W112" s="35">
         <f t="shared" ref="W112:AE112" si="20">SUM(W102:W111)</f>
         <v>7.8333333333333339</v>
       </c>
-      <c r="X112" s="16">
+      <c r="X112" s="35">
         <f t="shared" si="20"/>
         <v>11.333333333333334</v>
       </c>
-      <c r="Y112" s="16">
+      <c r="Y112" s="35">
         <f t="shared" si="20"/>
         <v>20.5</v>
       </c>
-      <c r="Z112" s="16">
+      <c r="Z112" s="35">
         <f t="shared" si="20"/>
         <v>21.166666666666664</v>
       </c>
-      <c r="AA112" s="16">
+      <c r="AA112" s="35">
         <f t="shared" si="20"/>
         <v>22</v>
       </c>
-      <c r="AB112" s="16">
+      <c r="AB112" s="35">
         <f t="shared" si="20"/>
         <v>4.25</v>
       </c>
-      <c r="AC112" s="16">
+      <c r="AC112" s="35">
         <f t="shared" si="20"/>
         <v>6.1666666666666661</v>
       </c>
-      <c r="AD112" s="16">
+      <c r="AD112" s="35">
         <f t="shared" si="20"/>
         <v>10.166666666666668</v>
       </c>
-      <c r="AE112" s="16">
+      <c r="AE112" s="35">
         <f t="shared" si="20"/>
         <v>19.333333333333332</v>
       </c>
@@ -3344,19 +3401,19 @@
       <c r="Z119" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AA119" s="28" t="s">
+      <c r="AA119" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AB119" s="28" t="s">
+      <c r="AB119" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="AC119" s="28" t="s">
+      <c r="AC119" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AD119" s="28" t="s">
+      <c r="AD119" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="AE119" s="28" t="s">
+      <c r="AE119" s="36" t="s">
         <v>29</v>
       </c>
       <c r="AF119" s="16" t="s">
@@ -3387,23 +3444,23 @@
         <f t="shared" si="21"/>
         <v>9.4488188976377965E-2</v>
       </c>
-      <c r="AA120" s="12">
+      <c r="AA120" s="8">
         <f t="shared" si="21"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="AB120" s="12">
+      <c r="AB120" s="8">
         <f t="shared" si="21"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="AC120" s="12">
+      <c r="AC120" s="8">
         <f t="shared" si="21"/>
         <v>5.4054054054054057E-2</v>
       </c>
-      <c r="AD120" s="12">
+      <c r="AD120" s="8">
         <f t="shared" si="21"/>
         <v>3.2786885245901634E-2</v>
       </c>
-      <c r="AE120" s="12">
+      <c r="AE120" s="8">
         <f t="shared" si="21"/>
         <v>7.7586206896551727E-2</v>
       </c>
@@ -3436,23 +3493,23 @@
         <f t="shared" si="22"/>
         <v>0.14173228346456695</v>
       </c>
-      <c r="AA121" s="12">
+      <c r="AA121" s="8">
         <f t="shared" si="22"/>
         <v>0.13636363636363635</v>
       </c>
-      <c r="AB121" s="12">
+      <c r="AB121" s="8">
         <f t="shared" si="22"/>
         <v>0.11764705882352941</v>
       </c>
-      <c r="AC121" s="12">
+      <c r="AC121" s="8">
         <f t="shared" si="22"/>
         <v>8.1081081081081086E-2</v>
       </c>
-      <c r="AD121" s="12">
+      <c r="AD121" s="8">
         <f t="shared" si="22"/>
         <v>0.14754098360655735</v>
       </c>
-      <c r="AE121" s="12">
+      <c r="AE121" s="8">
         <f t="shared" si="22"/>
         <v>0.15517241379310345</v>
       </c>
@@ -3485,23 +3542,23 @@
         <f t="shared" si="24"/>
         <v>0.14173228346456695</v>
       </c>
-      <c r="AA122" s="12">
+      <c r="AA122" s="8">
         <f t="shared" si="24"/>
         <v>0.13636363636363635</v>
       </c>
-      <c r="AB122" s="12">
+      <c r="AB122" s="8">
         <f t="shared" si="24"/>
         <v>7.8431372549019607E-2</v>
       </c>
-      <c r="AC122" s="12">
+      <c r="AC122" s="8">
         <f t="shared" si="24"/>
         <v>8.1081081081081086E-2</v>
       </c>
-      <c r="AD122" s="12">
+      <c r="AD122" s="8">
         <f t="shared" si="24"/>
         <v>6.5573770491803268E-2</v>
       </c>
-      <c r="AE122" s="12">
+      <c r="AE122" s="8">
         <f t="shared" si="24"/>
         <v>0.15517241379310345</v>
       </c>
@@ -3534,23 +3591,23 @@
         <f t="shared" si="25"/>
         <v>9.4488188976377965E-2</v>
       </c>
-      <c r="AA123" s="12">
+      <c r="AA123" s="8">
         <f t="shared" si="25"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="AB123" s="12">
+      <c r="AB123" s="8">
         <f t="shared" si="25"/>
         <v>7.8431372549019607E-2</v>
       </c>
-      <c r="AC123" s="12">
+      <c r="AC123" s="8">
         <f t="shared" si="25"/>
         <v>5.4054054054054057E-2</v>
       </c>
-      <c r="AD123" s="12">
+      <c r="AD123" s="8">
         <f t="shared" si="25"/>
         <v>3.2786885245901634E-2</v>
       </c>
-      <c r="AE123" s="12">
+      <c r="AE123" s="8">
         <f t="shared" si="25"/>
         <v>2.5862068965517244E-2</v>
       </c>
@@ -3583,23 +3640,23 @@
         <f t="shared" si="26"/>
         <v>4.7244094488188983E-2</v>
       </c>
-      <c r="AA124" s="12">
+      <c r="AA124" s="8">
         <f t="shared" si="26"/>
         <v>6.8181818181818177E-2</v>
       </c>
-      <c r="AB124" s="12">
+      <c r="AB124" s="8">
         <f t="shared" si="26"/>
         <v>7.8431372549019607E-2</v>
       </c>
-      <c r="AC124" s="12">
+      <c r="AC124" s="8">
         <f t="shared" si="26"/>
         <v>5.4054054054054057E-2</v>
       </c>
-      <c r="AD124" s="12">
+      <c r="AD124" s="8">
         <f t="shared" si="26"/>
         <v>4.9180327868852451E-2</v>
       </c>
-      <c r="AE124" s="12">
+      <c r="AE124" s="8">
         <f t="shared" si="26"/>
         <v>3.4482758620689655E-2</v>
       </c>
@@ -3609,46 +3666,46 @@
       </c>
     </row>
     <row r="125" spans="21:32" ht="21" x14ac:dyDescent="0.3">
-      <c r="U125" s="27" t="s">
+      <c r="U125" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="V125" s="12">
+      <c r="V125" s="8">
         <f>V107/V112</f>
         <v>2.7272727272727268E-2</v>
       </c>
-      <c r="W125" s="12">
+      <c r="W125" s="8">
         <f>W107/W112</f>
         <v>4.2553191489361694E-2</v>
       </c>
-      <c r="X125" s="12">
+      <c r="X125" s="8">
         <f t="shared" ref="X125:AE125" si="27">X107/X112</f>
         <v>2.9411764705882349E-2</v>
       </c>
-      <c r="Y125" s="12">
+      <c r="Y125" s="8">
         <f t="shared" si="27"/>
         <v>2.4390243902439025E-2</v>
       </c>
-      <c r="Z125" s="12">
+      <c r="Z125" s="8">
         <f t="shared" si="27"/>
         <v>3.1496062992125984E-2</v>
       </c>
-      <c r="AA125" s="12">
+      <c r="AA125" s="8">
         <f t="shared" si="27"/>
         <v>4.5454545454545456E-2</v>
       </c>
-      <c r="AB125" s="12">
+      <c r="AB125" s="8">
         <f t="shared" si="27"/>
         <v>7.8431372549019607E-2</v>
       </c>
-      <c r="AC125" s="12">
+      <c r="AC125" s="8">
         <f t="shared" si="27"/>
         <v>5.4054054054054057E-2</v>
       </c>
-      <c r="AD125" s="12">
+      <c r="AD125" s="8">
         <f t="shared" si="27"/>
         <v>4.9180327868852451E-2</v>
       </c>
-      <c r="AE125" s="12">
+      <c r="AE125" s="8">
         <f t="shared" si="27"/>
         <v>3.4482758620689655E-2</v>
       </c>
@@ -3658,46 +3715,46 @@
       </c>
     </row>
     <row r="126" spans="21:32" ht="21" x14ac:dyDescent="0.3">
-      <c r="U126" s="27" t="s">
+      <c r="U126" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="V126" s="12">
+      <c r="V126" s="8">
         <f>V108/V112</f>
         <v>0.21818181818181814</v>
       </c>
-      <c r="W126" s="12">
+      <c r="W126" s="8">
         <f>W108/W112</f>
         <v>0.25531914893617019</v>
       </c>
-      <c r="X126" s="12">
+      <c r="X126" s="8">
         <f t="shared" ref="X126:AE126" si="28">X108/X112</f>
         <v>0.26470588235294118</v>
       </c>
-      <c r="Y126" s="12">
+      <c r="Y126" s="8">
         <f t="shared" si="28"/>
         <v>0.14634146341463414</v>
       </c>
-      <c r="Z126" s="12">
+      <c r="Z126" s="8">
         <f t="shared" si="28"/>
         <v>0.14173228346456695</v>
       </c>
-      <c r="AA126" s="12">
+      <c r="AA126" s="8">
         <f t="shared" si="28"/>
         <v>0.13636363636363635</v>
       </c>
-      <c r="AB126" s="12">
+      <c r="AB126" s="8">
         <f t="shared" si="28"/>
         <v>0.23529411764705882</v>
       </c>
-      <c r="AC126" s="12">
+      <c r="AC126" s="8">
         <f t="shared" si="28"/>
         <v>0.32432432432432434</v>
       </c>
-      <c r="AD126" s="12">
+      <c r="AD126" s="8">
         <f t="shared" si="28"/>
         <v>0.29508196721311469</v>
       </c>
-      <c r="AE126" s="12">
+      <c r="AE126" s="8">
         <f t="shared" si="28"/>
         <v>0.15517241379310345</v>
       </c>
@@ -3707,46 +3764,46 @@
       </c>
     </row>
     <row r="127" spans="21:32" ht="21" x14ac:dyDescent="0.3">
-      <c r="U127" s="27" t="s">
+      <c r="U127" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="V127" s="12">
+      <c r="V127" s="8">
         <f>V109/V112</f>
         <v>0.16363636363636361</v>
       </c>
-      <c r="W127" s="12">
+      <c r="W127" s="8">
         <f>W109/W112</f>
         <v>0.25531914893617019</v>
       </c>
-      <c r="X127" s="12">
+      <c r="X127" s="8">
         <f t="shared" ref="X127:AE127" si="29">X109/X112</f>
         <v>0.1764705882352941</v>
       </c>
-      <c r="Y127" s="12">
+      <c r="Y127" s="8">
         <f t="shared" si="29"/>
         <v>0.14634146341463414</v>
       </c>
-      <c r="Z127" s="12">
+      <c r="Z127" s="8">
         <f t="shared" si="29"/>
         <v>0.14173228346456695</v>
       </c>
-      <c r="AA127" s="12">
+      <c r="AA127" s="8">
         <f t="shared" si="29"/>
         <v>0.13636363636363635</v>
       </c>
-      <c r="AB127" s="12">
+      <c r="AB127" s="8">
         <f t="shared" si="29"/>
         <v>0.11764705882352941</v>
       </c>
-      <c r="AC127" s="12">
+      <c r="AC127" s="8">
         <f t="shared" si="29"/>
         <v>0.16216216216216217</v>
       </c>
-      <c r="AD127" s="12">
+      <c r="AD127" s="8">
         <f t="shared" si="29"/>
         <v>0.1967213114754098</v>
       </c>
-      <c r="AE127" s="12">
+      <c r="AE127" s="8">
         <f t="shared" si="29"/>
         <v>0.15517241379310345</v>
       </c>
@@ -3756,46 +3813,46 @@
       </c>
     </row>
     <row r="128" spans="21:32" ht="21" x14ac:dyDescent="0.3">
-      <c r="U128" s="27" t="s">
+      <c r="U128" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="V128" s="12">
+      <c r="V128" s="8">
         <f>V110/V112</f>
         <v>0.16363636363636361</v>
       </c>
-      <c r="W128" s="12">
+      <c r="W128" s="8">
         <f>W110/W112</f>
         <v>8.5106382978723388E-2</v>
       </c>
-      <c r="X128" s="12">
+      <c r="X128" s="8">
         <f t="shared" ref="X128:AE128" si="30">X110/X112</f>
         <v>0.13235294117647059</v>
       </c>
-      <c r="Y128" s="12">
+      <c r="Y128" s="8">
         <f t="shared" si="30"/>
         <v>0.14634146341463414</v>
       </c>
-      <c r="Z128" s="12">
+      <c r="Z128" s="8">
         <f t="shared" si="30"/>
         <v>9.4488188976377965E-2</v>
       </c>
-      <c r="AA128" s="12">
+      <c r="AA128" s="8">
         <f t="shared" si="30"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="AB128" s="12">
+      <c r="AB128" s="8">
         <f t="shared" si="30"/>
         <v>7.8431372549019607E-2</v>
       </c>
-      <c r="AC128" s="12">
+      <c r="AC128" s="8">
         <f t="shared" si="30"/>
         <v>8.1081081081081086E-2</v>
       </c>
-      <c r="AD128" s="12">
+      <c r="AD128" s="8">
         <f t="shared" si="30"/>
         <v>9.8360655737704902E-2</v>
       </c>
-      <c r="AE128" s="12">
+      <c r="AE128" s="8">
         <f t="shared" si="30"/>
         <v>0.15517241379310345</v>
       </c>
@@ -3805,46 +3862,46 @@
       </c>
     </row>
     <row r="129" spans="21:34" ht="21" x14ac:dyDescent="0.3">
-      <c r="U129" s="27" t="s">
+      <c r="U129" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="V129" s="12">
+      <c r="V129" s="8">
         <f>V111/V112</f>
         <v>3.6363636363636355E-2</v>
       </c>
-      <c r="W129" s="12">
+      <c r="W129" s="8">
         <f>W111/W112</f>
         <v>4.2553191489361694E-2</v>
       </c>
-      <c r="X129" s="12">
+      <c r="X129" s="8">
         <f t="shared" ref="X129:AE129" si="31">X111/X112</f>
         <v>2.9411764705882349E-2</v>
       </c>
-      <c r="Y129" s="12">
+      <c r="Y129" s="8">
         <f t="shared" si="31"/>
         <v>9.7560975609756101E-2</v>
       </c>
-      <c r="Z129" s="12">
+      <c r="Z129" s="8">
         <f t="shared" si="31"/>
         <v>7.0866141732283477E-2</v>
       </c>
-      <c r="AA129" s="12">
+      <c r="AA129" s="8">
         <f t="shared" si="31"/>
         <v>6.8181818181818177E-2</v>
       </c>
-      <c r="AB129" s="12">
+      <c r="AB129" s="8">
         <f t="shared" si="31"/>
         <v>7.8431372549019607E-2</v>
       </c>
-      <c r="AC129" s="12">
+      <c r="AC129" s="8">
         <f t="shared" si="31"/>
         <v>5.4054054054054057E-2</v>
       </c>
-      <c r="AD129" s="12">
+      <c r="AD129" s="8">
         <f t="shared" si="31"/>
         <v>3.2786885245901634E-2</v>
       </c>
-      <c r="AE129" s="12">
+      <c r="AE129" s="8">
         <f t="shared" si="31"/>
         <v>5.1724137931034489E-2</v>
       </c>
@@ -3854,17 +3911,17 @@
       </c>
     </row>
     <row r="130" spans="21:34" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="U130" s="15"/>
-      <c r="V130" s="14"/>
-      <c r="W130" s="14"/>
-      <c r="X130" s="14"/>
-      <c r="Y130" s="14"/>
-      <c r="Z130" s="14"/>
-      <c r="AA130" s="14"/>
-      <c r="AB130" s="14"/>
-      <c r="AC130" s="14"/>
-      <c r="AD130" s="14"/>
-      <c r="AE130" s="14"/>
+      <c r="U130" s="32"/>
+      <c r="V130" s="33"/>
+      <c r="W130" s="33"/>
+      <c r="X130" s="33"/>
+      <c r="Y130" s="33"/>
+      <c r="Z130" s="33"/>
+      <c r="AA130" s="33"/>
+      <c r="AB130" s="33"/>
+      <c r="AC130" s="33"/>
+      <c r="AD130" s="33"/>
+      <c r="AE130" s="33"/>
     </row>
     <row r="134" spans="21:34" ht="36" x14ac:dyDescent="0.3">
       <c r="U134" s="11" t="s">
@@ -8197,8 +8254,214 @@
         <v>7</v>
       </c>
     </row>
+    <row r="299" spans="21:28" ht="21" x14ac:dyDescent="0.3">
+      <c r="U299" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="V299" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="W299" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="X299" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y299" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA299" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB299" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="300" spans="21:28" ht="21" x14ac:dyDescent="0.3">
+      <c r="U300" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="V300" s="23">
+        <f>AF102</f>
+        <v>0</v>
+      </c>
+      <c r="W300" s="23">
+        <f>AF157</f>
+        <v>0</v>
+      </c>
+      <c r="X300" s="23">
+        <f>AF212</f>
+        <v>0</v>
+      </c>
+      <c r="Y300" s="23">
+        <f>AF268</f>
+        <v>0</v>
+      </c>
+      <c r="AA300" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB300" s="1">
+        <v>0.48445974378513695</v>
+      </c>
+    </row>
+    <row r="301" spans="21:28" ht="21" x14ac:dyDescent="0.3">
+      <c r="U301" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="V301" s="23">
+        <f t="shared" ref="V301:V303" si="69">AF103</f>
+        <v>0</v>
+      </c>
+      <c r="W301" s="23">
+        <f t="shared" ref="W301:W303" si="70">AF158</f>
+        <v>0</v>
+      </c>
+      <c r="X301" s="23">
+        <f t="shared" ref="X301:X303" si="71">AF213</f>
+        <v>0</v>
+      </c>
+      <c r="Y301" s="23">
+        <f t="shared" ref="Y301:Y303" si="72">AF269</f>
+        <v>0</v>
+      </c>
+      <c r="AA301" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB301" s="1">
+        <v>4.7622047882677349E-2</v>
+      </c>
+    </row>
+    <row r="302" spans="21:28" ht="21" x14ac:dyDescent="0.3">
+      <c r="U302" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="V302" s="23">
+        <f t="shared" si="69"/>
+        <v>0</v>
+      </c>
+      <c r="W302" s="23">
+        <f t="shared" si="70"/>
+        <v>0</v>
+      </c>
+      <c r="X302" s="23">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="Y302" s="23">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="AA302" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB302" s="1">
+        <v>0.36612693071609786</v>
+      </c>
+    </row>
+    <row r="303" spans="21:28" ht="21" x14ac:dyDescent="0.3">
+      <c r="U303" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="V303" s="23">
+        <f t="shared" si="69"/>
+        <v>0</v>
+      </c>
+      <c r="W303" s="23">
+        <f t="shared" si="70"/>
+        <v>0</v>
+      </c>
+      <c r="X303" s="23">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="Y303" s="23">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="AA303" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB303" s="1">
+        <v>0.10179127761608781</v>
+      </c>
+    </row>
+    <row r="308" spans="21:23" ht="21" x14ac:dyDescent="0.3">
+      <c r="U308" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="V308" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="W308" s="25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="309" spans="21:23" ht="21" x14ac:dyDescent="0.3">
+      <c r="U309" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="V309" s="23" t="e">
+        <f>MMULT(V294:Y294,AB294:AB297)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W309" s="26" t="e">
+        <f>RANK(V309,V309:V318,0)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="310" spans="21:23" ht="21" x14ac:dyDescent="0.3">
+      <c r="U310" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="V310" s="23" t="e">
+        <f>MMULT(V295:Y295,AB294:AB297)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W310" s="26" t="e">
+        <f>RANK(V310,V309:V318,0)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="311" spans="21:23" ht="21" x14ac:dyDescent="0.3">
+      <c r="U311" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="V311" s="23" t="e">
+        <f>MMULT(V296:Y296,AB294:AB297)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W311" s="26" t="e">
+        <f>RANK(V311,V309:V318,0)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="312" spans="21:23" ht="21" x14ac:dyDescent="0.3">
+      <c r="U312" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="V312" s="23" t="e">
+        <f>MMULT(V297:Y297,AB294:AB297)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W312" s="26" t="e">
+        <f>RANK(V312,V309:V318,0)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AF258:AG258"/>
+    <mergeCell ref="AF259:AG259"/>
+    <mergeCell ref="AF201:AG201"/>
+    <mergeCell ref="AF202:AG202"/>
+    <mergeCell ref="AF203:AG203"/>
+    <mergeCell ref="AF256:AG256"/>
+    <mergeCell ref="AF257:AG257"/>
+    <mergeCell ref="AF145:AG145"/>
+    <mergeCell ref="AF146:AG146"/>
+    <mergeCell ref="AF147:AG147"/>
+    <mergeCell ref="AF148:AG148"/>
+    <mergeCell ref="AF200:AG200"/>
     <mergeCell ref="AF90:AG90"/>
     <mergeCell ref="AF91:AG91"/>
     <mergeCell ref="AF92:AG92"/>
@@ -8207,18 +8470,6 @@
     <mergeCell ref="M40:N40"/>
     <mergeCell ref="M41:N41"/>
     <mergeCell ref="M42:N42"/>
-    <mergeCell ref="AF145:AG145"/>
-    <mergeCell ref="AF146:AG146"/>
-    <mergeCell ref="AF147:AG147"/>
-    <mergeCell ref="AF148:AG148"/>
-    <mergeCell ref="AF200:AG200"/>
-    <mergeCell ref="AF258:AG258"/>
-    <mergeCell ref="AF259:AG259"/>
-    <mergeCell ref="AF201:AG201"/>
-    <mergeCell ref="AF202:AG202"/>
-    <mergeCell ref="AF203:AG203"/>
-    <mergeCell ref="AF256:AG256"/>
-    <mergeCell ref="AF257:AG257"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8226,4 +8477,338 @@
     <ignoredError sqref="W143 AD141:AD144 AF141:AH144 AH145 AH147" evalError="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E685A3B-2712-4D4E-B3A3-A2F89ADEC8D7}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="108" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="54" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="F2" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="108" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="12">
+        <v>3</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2</v>
+      </c>
+      <c r="E3" s="12">
+        <v>3</v>
+      </c>
+      <c r="F3" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="38">
+        <f>SUM(B2:B6)</f>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="C7" s="38">
+        <f t="shared" ref="C7:F7" si="0">SUM(C2:C6)</f>
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="38">
+        <f t="shared" si="0"/>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="E7" s="38">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F7" s="38">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="40">
+        <f>B2/$B$7</f>
+        <v>0.13953488372093023</v>
+      </c>
+      <c r="C13" s="12">
+        <f t="shared" ref="C13:F13" si="1">C2/C7</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E13" s="12">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="1"/>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="G13" s="39">
+        <f>AVERAGE(B13:F13)</f>
+        <v>0.14827061310782241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="12">
+        <f t="shared" ref="B14:F17" si="2">B3/$B$7</f>
+        <v>0.41860465116279066</v>
+      </c>
+      <c r="C14" s="12">
+        <f t="shared" si="2"/>
+        <v>0.13953488372093023</v>
+      </c>
+      <c r="D14" s="12">
+        <f t="shared" si="2"/>
+        <v>0.27906976744186046</v>
+      </c>
+      <c r="E14" s="12">
+        <f t="shared" si="2"/>
+        <v>0.41860465116279066</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="2"/>
+        <v>0.41860465116279066</v>
+      </c>
+      <c r="G14" s="39">
+        <f t="shared" ref="G14:G17" si="3">AVERAGE(B14:F14)</f>
+        <v>0.33488372093023255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="12">
+        <f t="shared" si="2"/>
+        <v>0.27906976744186046</v>
+      </c>
+      <c r="C15" s="12">
+        <f t="shared" si="2"/>
+        <v>6.9767441860465115E-2</v>
+      </c>
+      <c r="D15" s="12">
+        <f t="shared" si="2"/>
+        <v>0.13953488372093023</v>
+      </c>
+      <c r="E15" s="12">
+        <f t="shared" si="2"/>
+        <v>0.41860465116279066</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="2"/>
+        <v>0.41860465116279066</v>
+      </c>
+      <c r="G15" s="39">
+        <f t="shared" si="3"/>
+        <v>0.26511627906976742</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="12">
+        <f t="shared" si="2"/>
+        <v>9.3023255813953473E-2</v>
+      </c>
+      <c r="C16" s="12">
+        <f t="shared" si="2"/>
+        <v>4.6511627906976737E-2</v>
+      </c>
+      <c r="D16" s="12">
+        <f t="shared" si="2"/>
+        <v>4.6511627906976737E-2</v>
+      </c>
+      <c r="E16" s="12">
+        <f t="shared" si="2"/>
+        <v>0.13953488372093023</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="2"/>
+        <v>0.27906976744186046</v>
+      </c>
+      <c r="G16" s="39">
+        <f t="shared" si="3"/>
+        <v>0.12093023255813953</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="12">
+        <f t="shared" si="2"/>
+        <v>6.9767441860465115E-2</v>
+      </c>
+      <c r="C17" s="12">
+        <f t="shared" si="2"/>
+        <v>4.6511627906976737E-2</v>
+      </c>
+      <c r="D17" s="12">
+        <f t="shared" si="2"/>
+        <v>4.6511627906976737E-2</v>
+      </c>
+      <c r="E17" s="12">
+        <f t="shared" si="2"/>
+        <v>6.9767441860465115E-2</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="2"/>
+        <v>0.13953488372093023</v>
+      </c>
+      <c r="G17" s="39">
+        <f t="shared" si="3"/>
+        <v>7.441860465116279E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Done Code Logic AHP and Load Food to Popup
</commit_message>
<xml_diff>
--- a/AHP Sản phẩm Món chính.xlsx
+++ b/AHP Sản phẩm Món chính.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhokk\Desktop\HoTroRaQuyetDinh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164E3906-E2BB-433B-B3A1-AC39D3184B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91A5AB0-4B55-4A57-A0BB-E625A9AB209D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{738D0DCC-DACC-4475-BFCE-0371B9E87382}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{738D0DCC-DACC-4475-BFCE-0371B9E87382}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="32">
   <si>
     <t>Calo</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Bò xào lăn + Bánh mỳ</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>weight</t>
   </si>
 </sst>
 </file>
@@ -432,12 +438,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -464,6 +464,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -783,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8420C6-B896-437C-BDF8-F9FED97D9E93}">
   <dimension ref="C8:AH312"/>
   <sheetViews>
-    <sheetView topLeftCell="J92" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V116" sqref="V116"/>
+    <sheetView tabSelected="1" topLeftCell="Q266" zoomScale="57" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y282" sqref="Y282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,39 +1279,39 @@
       </c>
     </row>
     <row r="39" spans="8:31" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M39" s="30" t="s">
+      <c r="M39" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="N39" s="30"/>
+      <c r="N39" s="40"/>
       <c r="O39" s="9">
         <f>AVERAGE(O35:O38)</f>
         <v>4.1418161704801264</v>
       </c>
     </row>
     <row r="40" spans="8:31" x14ac:dyDescent="0.3">
-      <c r="M40" s="30" t="s">
+      <c r="M40" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="N40" s="30"/>
+      <c r="N40" s="40"/>
       <c r="O40" s="9">
         <v>0.9</v>
       </c>
     </row>
     <row r="41" spans="8:31" x14ac:dyDescent="0.3">
-      <c r="M41" s="30" t="s">
+      <c r="M41" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="N41" s="30"/>
+      <c r="N41" s="40"/>
       <c r="O41" s="13">
         <f>(O39-4)/3</f>
         <v>4.7272056826708798E-2</v>
       </c>
     </row>
     <row r="42" spans="8:31" x14ac:dyDescent="0.3">
-      <c r="M42" s="30" t="s">
+      <c r="M42" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="N42" s="30"/>
+      <c r="N42" s="40"/>
       <c r="O42" s="13">
         <f>O41/O40</f>
         <v>5.2524507585232E-2</v>
@@ -2898,39 +2904,39 @@
       </c>
     </row>
     <row r="90" spans="21:34" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AF90" s="29" t="s">
+      <c r="AF90" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="AG90" s="29"/>
+      <c r="AG90" s="39"/>
       <c r="AH90" s="19">
         <f>AVERAGE(AH80:AH89)</f>
         <v>10.692659816718891</v>
       </c>
     </row>
     <row r="91" spans="21:34" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AF91" s="29" t="s">
+      <c r="AF91" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="AG91" s="29"/>
+      <c r="AG91" s="39"/>
       <c r="AH91" s="19">
         <v>1.49</v>
       </c>
     </row>
     <row r="92" spans="21:34" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AF92" s="29" t="s">
+      <c r="AF92" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="AG92" s="29"/>
+      <c r="AG92" s="39"/>
       <c r="AH92" s="18">
         <f>(AH90-10)/9</f>
         <v>7.6962201857654511E-2</v>
       </c>
     </row>
     <row r="93" spans="21:34" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AF93" s="29" t="s">
+      <c r="AF93" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="AG93" s="29"/>
+      <c r="AG93" s="39"/>
       <c r="AH93" s="21">
         <f>AH92/AH91</f>
         <v>5.1652484468224506E-2</v>
@@ -2971,19 +2977,19 @@
       <c r="Z101" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AA101" s="36" t="s">
+      <c r="AA101" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="AB101" s="36" t="s">
+      <c r="AB101" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="AC101" s="36" t="s">
+      <c r="AC101" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="AD101" s="36" t="s">
+      <c r="AD101" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="AE101" s="36" t="s">
+      <c r="AE101" s="34" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3163,7 +3169,7 @@
       </c>
     </row>
     <row r="107" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="U107" s="31" t="s">
+      <c r="U107" s="29" t="s">
         <v>25</v>
       </c>
       <c r="V107" s="8">
@@ -3198,7 +3204,7 @@
       </c>
     </row>
     <row r="108" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="U108" s="31" t="s">
+      <c r="U108" s="29" t="s">
         <v>26</v>
       </c>
       <c r="V108" s="8">
@@ -3233,7 +3239,7 @@
       </c>
     </row>
     <row r="109" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="U109" s="31" t="s">
+      <c r="U109" s="29" t="s">
         <v>27</v>
       </c>
       <c r="V109" s="8">
@@ -3268,7 +3274,7 @@
       </c>
     </row>
     <row r="110" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="U110" s="31" t="s">
+      <c r="U110" s="29" t="s">
         <v>28</v>
       </c>
       <c r="V110" s="8">
@@ -3303,7 +3309,7 @@
       </c>
     </row>
     <row r="111" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="U111" s="31" t="s">
+      <c r="U111" s="29" t="s">
         <v>29</v>
       </c>
       <c r="V111" s="8">
@@ -3338,46 +3344,46 @@
       </c>
     </row>
     <row r="112" spans="21:34" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="U112" s="34" t="s">
+      <c r="U112" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="V112" s="35">
+      <c r="V112" s="33">
         <f>SUM(V102:V111)</f>
         <v>18.333333333333336</v>
       </c>
-      <c r="W112" s="35">
+      <c r="W112" s="33">
         <f t="shared" ref="W112:AE112" si="20">SUM(W102:W111)</f>
         <v>7.8333333333333339</v>
       </c>
-      <c r="X112" s="35">
+      <c r="X112" s="33">
         <f t="shared" si="20"/>
         <v>11.333333333333334</v>
       </c>
-      <c r="Y112" s="35">
+      <c r="Y112" s="33">
         <f t="shared" si="20"/>
         <v>20.5</v>
       </c>
-      <c r="Z112" s="35">
+      <c r="Z112" s="33">
         <f t="shared" si="20"/>
         <v>21.166666666666664</v>
       </c>
-      <c r="AA112" s="35">
+      <c r="AA112" s="33">
         <f t="shared" si="20"/>
         <v>22</v>
       </c>
-      <c r="AB112" s="35">
+      <c r="AB112" s="33">
         <f t="shared" si="20"/>
         <v>4.25</v>
       </c>
-      <c r="AC112" s="35">
+      <c r="AC112" s="33">
         <f t="shared" si="20"/>
         <v>6.1666666666666661</v>
       </c>
-      <c r="AD112" s="35">
+      <c r="AD112" s="33">
         <f t="shared" si="20"/>
         <v>10.166666666666668</v>
       </c>
-      <c r="AE112" s="35">
+      <c r="AE112" s="33">
         <f t="shared" si="20"/>
         <v>19.333333333333332</v>
       </c>
@@ -3401,19 +3407,19 @@
       <c r="Z119" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AA119" s="36" t="s">
+      <c r="AA119" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="AB119" s="36" t="s">
+      <c r="AB119" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="AC119" s="36" t="s">
+      <c r="AC119" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="AD119" s="36" t="s">
+      <c r="AD119" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="AE119" s="36" t="s">
+      <c r="AE119" s="34" t="s">
         <v>29</v>
       </c>
       <c r="AF119" s="16" t="s">
@@ -3666,7 +3672,7 @@
       </c>
     </row>
     <row r="125" spans="21:32" ht="21" x14ac:dyDescent="0.3">
-      <c r="U125" s="31" t="s">
+      <c r="U125" s="29" t="s">
         <v>25</v>
       </c>
       <c r="V125" s="8">
@@ -3715,7 +3721,7 @@
       </c>
     </row>
     <row r="126" spans="21:32" ht="21" x14ac:dyDescent="0.3">
-      <c r="U126" s="31" t="s">
+      <c r="U126" s="29" t="s">
         <v>26</v>
       </c>
       <c r="V126" s="8">
@@ -3764,7 +3770,7 @@
       </c>
     </row>
     <row r="127" spans="21:32" ht="21" x14ac:dyDescent="0.3">
-      <c r="U127" s="31" t="s">
+      <c r="U127" s="29" t="s">
         <v>27</v>
       </c>
       <c r="V127" s="8">
@@ -3813,7 +3819,7 @@
       </c>
     </row>
     <row r="128" spans="21:32" ht="21" x14ac:dyDescent="0.3">
-      <c r="U128" s="31" t="s">
+      <c r="U128" s="29" t="s">
         <v>28</v>
       </c>
       <c r="V128" s="8">
@@ -3862,7 +3868,7 @@
       </c>
     </row>
     <row r="129" spans="21:34" ht="21" x14ac:dyDescent="0.3">
-      <c r="U129" s="31" t="s">
+      <c r="U129" s="29" t="s">
         <v>29</v>
       </c>
       <c r="V129" s="8">
@@ -3911,17 +3917,17 @@
       </c>
     </row>
     <row r="130" spans="21:34" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="U130" s="32"/>
-      <c r="V130" s="33"/>
-      <c r="W130" s="33"/>
-      <c r="X130" s="33"/>
-      <c r="Y130" s="33"/>
-      <c r="Z130" s="33"/>
-      <c r="AA130" s="33"/>
-      <c r="AB130" s="33"/>
-      <c r="AC130" s="33"/>
-      <c r="AD130" s="33"/>
-      <c r="AE130" s="33"/>
+      <c r="U130" s="30"/>
+      <c r="V130" s="31"/>
+      <c r="W130" s="31"/>
+      <c r="X130" s="31"/>
+      <c r="Y130" s="31"/>
+      <c r="Z130" s="31"/>
+      <c r="AA130" s="31"/>
+      <c r="AB130" s="31"/>
+      <c r="AC130" s="31"/>
+      <c r="AD130" s="31"/>
+      <c r="AE130" s="31"/>
     </row>
     <row r="134" spans="21:34" ht="36" x14ac:dyDescent="0.3">
       <c r="U134" s="11" t="s">
@@ -4538,39 +4544,39 @@
       </c>
     </row>
     <row r="145" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF145" s="29" t="s">
+      <c r="AF145" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="AG145" s="29"/>
+      <c r="AG145" s="39"/>
       <c r="AH145" s="19">
         <f>AVERAGE(AH135:AH144)</f>
         <v>10.501230269611817</v>
       </c>
     </row>
     <row r="146" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF146" s="29" t="s">
+      <c r="AF146" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="AG146" s="29"/>
+      <c r="AG146" s="39"/>
       <c r="AH146" s="19">
         <v>1.49</v>
       </c>
     </row>
     <row r="147" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF147" s="29" t="s">
+      <c r="AF147" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="AG147" s="29"/>
+      <c r="AG147" s="39"/>
       <c r="AH147" s="18">
         <f>(AH145-10)/9</f>
         <v>5.5692252179090768E-2</v>
       </c>
     </row>
     <row r="148" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF148" s="29" t="s">
+      <c r="AF148" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="AG148" s="29"/>
+      <c r="AG148" s="39"/>
       <c r="AH148" s="21">
         <f>AH147/AH146</f>
         <v>3.7377350455765616E-2</v>
@@ -6178,39 +6184,39 @@
       </c>
     </row>
     <row r="200" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF200" s="29" t="s">
+      <c r="AF200" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="AG200" s="29"/>
+      <c r="AG200" s="39"/>
       <c r="AH200" s="19">
         <f>AVERAGE(AH190:AH199)</f>
         <v>10.328750529286776</v>
       </c>
     </row>
     <row r="201" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF201" s="29" t="s">
+      <c r="AF201" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="AG201" s="29"/>
+      <c r="AG201" s="39"/>
       <c r="AH201" s="19">
         <v>1.49</v>
       </c>
     </row>
     <row r="202" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF202" s="29" t="s">
+      <c r="AF202" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="AG202" s="29"/>
+      <c r="AG202" s="39"/>
       <c r="AH202" s="18">
         <f>(AH200-10)/9</f>
         <v>3.652783658741951E-2</v>
       </c>
     </row>
     <row r="203" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF203" s="29" t="s">
+      <c r="AF203" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="AG203" s="29"/>
+      <c r="AG203" s="39"/>
       <c r="AH203" s="21">
         <f>AH202/AH201</f>
         <v>2.4515326568737925E-2</v>
@@ -7818,39 +7824,39 @@
       </c>
     </row>
     <row r="256" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF256" s="29" t="s">
+      <c r="AF256" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="AG256" s="29"/>
+      <c r="AG256" s="39"/>
       <c r="AH256" s="19">
         <f>AVERAGE(AH246:AH255)</f>
         <v>10.414035519086914</v>
       </c>
     </row>
     <row r="257" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF257" s="29" t="s">
+      <c r="AF257" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="AG257" s="29"/>
+      <c r="AG257" s="39"/>
       <c r="AH257" s="19">
         <v>1.49</v>
       </c>
     </row>
     <row r="258" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF258" s="29" t="s">
+      <c r="AF258" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="AG258" s="29"/>
+      <c r="AG258" s="39"/>
       <c r="AH258" s="18">
         <f>(AH256-10)/9</f>
         <v>4.6003946565212672E-2</v>
       </c>
     </row>
     <row r="259" spans="21:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="AF259" s="29" t="s">
+      <c r="AF259" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="AG259" s="29"/>
+      <c r="AG259" s="39"/>
       <c r="AH259" s="21">
         <f>AH258/AH257</f>
         <v>3.0875131922961527E-2</v>
@@ -8450,18 +8456,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AF258:AG258"/>
-    <mergeCell ref="AF259:AG259"/>
-    <mergeCell ref="AF201:AG201"/>
-    <mergeCell ref="AF202:AG202"/>
-    <mergeCell ref="AF203:AG203"/>
-    <mergeCell ref="AF256:AG256"/>
-    <mergeCell ref="AF257:AG257"/>
-    <mergeCell ref="AF145:AG145"/>
-    <mergeCell ref="AF146:AG146"/>
-    <mergeCell ref="AF147:AG147"/>
-    <mergeCell ref="AF148:AG148"/>
-    <mergeCell ref="AF200:AG200"/>
     <mergeCell ref="AF90:AG90"/>
     <mergeCell ref="AF91:AG91"/>
     <mergeCell ref="AF92:AG92"/>
@@ -8470,6 +8464,18 @@
     <mergeCell ref="M40:N40"/>
     <mergeCell ref="M41:N41"/>
     <mergeCell ref="M42:N42"/>
+    <mergeCell ref="AF145:AG145"/>
+    <mergeCell ref="AF146:AG146"/>
+    <mergeCell ref="AF147:AG147"/>
+    <mergeCell ref="AF148:AG148"/>
+    <mergeCell ref="AF200:AG200"/>
+    <mergeCell ref="AF258:AG258"/>
+    <mergeCell ref="AF259:AG259"/>
+    <mergeCell ref="AF201:AG201"/>
+    <mergeCell ref="AF202:AG202"/>
+    <mergeCell ref="AF203:AG203"/>
+    <mergeCell ref="AF256:AG256"/>
+    <mergeCell ref="AF257:AG257"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8481,10 +8487,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E685A3B-2712-4D4E-B3A3-A2F89ADEC8D7}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8497,7 +8503,7 @@
     <col min="6" max="6" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="108" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="54" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -8516,8 +8522,18 @@
       <c r="F1" s="28" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="54" x14ac:dyDescent="0.3">
+      <c r="O1" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1">
+        <f>MMULT(K11:N11,R11:R14)</f>
+        <v>0.21732096108564508</v>
+      </c>
+      <c r="Q1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="108" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>20</v>
       </c>
@@ -8528,16 +8544,26 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D2" s="12">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E2" s="12">
-        <v>1.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F2" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="108" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2">
+        <f>MMULT(K12:N12,R11:R14)</f>
+        <v>0.19748300480093944</v>
+      </c>
+      <c r="Q2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>21</v>
       </c>
@@ -8548,101 +8574,162 @@
         <v>1</v>
       </c>
       <c r="D3" s="12">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E3" s="12">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="F3" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="O3" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3">
+        <f>MMULT(K13:N13,R11:R14)</f>
+        <v>0.27416483869477615</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="90" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4" s="12">
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
       </c>
       <c r="E4" s="12">
-        <v>3</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F4" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="O4" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4">
+        <f>MMULT(K14:N14,R11:R14)</f>
+        <v>0.13417487101811071</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="90" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="12">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C5" s="12">
-        <v>0.33333333333333331</v>
-      </c>
       <c r="D5" s="12">
-        <v>0.33333333333333331</v>
+        <v>1.5</v>
       </c>
       <c r="E5" s="12">
         <v>1</v>
       </c>
       <c r="F5" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="O5" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5">
+        <f>MMULT(K15:N15,R11:R14)</f>
+        <v>0.17685632440052859</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="36" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="12">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C6" s="12">
-        <v>0.33333333333333331</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="D6" s="12">
-        <v>0.33333333333333331</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="E6" s="12">
-        <v>0.5</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="F6" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="38">
+      <c r="B7" s="36">
         <f>SUM(B2:B6)</f>
-        <v>7.166666666666667</v>
-      </c>
-      <c r="C7" s="38">
+        <v>11.2</v>
+      </c>
+      <c r="C7" s="36">
         <f t="shared" ref="C7:F7" si="0">SUM(C2:C6)</f>
-        <v>2.5</v>
-      </c>
-      <c r="D7" s="38">
+        <v>2.8095238095238093</v>
+      </c>
+      <c r="D7" s="36">
         <f t="shared" si="0"/>
-        <v>4.166666666666667</v>
-      </c>
-      <c r="E7" s="38">
+        <v>4.3928571428571432</v>
+      </c>
+      <c r="E7" s="36">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="F7" s="38">
+        <v>3.6428571428571428</v>
+      </c>
+      <c r="F7" s="36">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <v>0.33828490643906467</v>
+      </c>
+      <c r="L11">
+        <v>0.14827061310782241</v>
+      </c>
+      <c r="M11">
+        <v>9.6551242236024848E-2</v>
+      </c>
+      <c r="N11">
+        <v>0.10830576086941139</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.48445974378513695</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="36" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>1</v>
       </c>
@@ -8661,150 +8748,368 @@
       <c r="F12" s="28" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="K12">
+        <v>0.10763898035703309</v>
+      </c>
+      <c r="L12">
+        <v>0.38093305144467932</v>
+      </c>
+      <c r="M12">
+        <v>0.25642391304347828</v>
+      </c>
+      <c r="N12">
+        <v>0.32725534520454641</v>
+      </c>
+      <c r="R12" s="1">
+        <v>4.7622047882677349E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="36" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="40">
+      <c r="B13" s="38">
         <f>B2/$B$7</f>
-        <v>0.13953488372093023</v>
+        <v>8.9285714285714288E-2</v>
       </c>
       <c r="C13" s="12">
-        <f t="shared" ref="C13:F13" si="1">C2/C7</f>
-        <v>0.13333333333333333</v>
+        <f>C2/$C$7</f>
+        <v>0.11864406779661017</v>
       </c>
       <c r="D13" s="12">
-        <f t="shared" si="1"/>
-        <v>0.12</v>
+        <f>D2/$D$7</f>
+        <v>5.6910569105691054E-2</v>
       </c>
       <c r="E13" s="12">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <f>E2/$E$7</f>
+        <v>9.1503267973856203E-2</v>
       </c>
       <c r="F13" s="12">
-        <f t="shared" si="1"/>
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="G13" s="39">
+        <f>F2/$F$7</f>
+        <v>0.18518518518518517</v>
+      </c>
+      <c r="G13" s="37">
         <f>AVERAGE(B13:F13)</f>
-        <v>0.14827061310782241</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+        <v>0.10830576086941139</v>
+      </c>
+      <c r="K13">
+        <v>0.1753747266931851</v>
+      </c>
+      <c r="L13">
+        <v>0.26502607470049327</v>
+      </c>
+      <c r="M13">
+        <v>0.41199378881987575</v>
+      </c>
+      <c r="N13">
+        <v>0.25286781287316268</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0.36612693071609786</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="36" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="12">
-        <f t="shared" ref="B14:F17" si="2">B3/$B$7</f>
-        <v>0.41860465116279066</v>
+        <f t="shared" ref="B14:F17" si="1">B3/$B$7</f>
+        <v>0.26785714285714285</v>
       </c>
       <c r="C14" s="12">
-        <f t="shared" si="2"/>
-        <v>0.13953488372093023</v>
+        <f t="shared" ref="C14:C17" si="2">C3/$C$7</f>
+        <v>0.35593220338983056</v>
       </c>
       <c r="D14" s="12">
-        <f t="shared" si="2"/>
-        <v>0.27906976744186046</v>
+        <f t="shared" ref="D14:D17" si="3">D3/$D$7</f>
+        <v>0.34146341463414631</v>
       </c>
       <c r="E14" s="12">
-        <f t="shared" si="2"/>
-        <v>0.41860465116279066</v>
+        <f t="shared" ref="E14:E17" si="4">E3/$E$7</f>
+        <v>0.41176470588235292</v>
       </c>
       <c r="F14" s="12">
-        <f t="shared" si="2"/>
-        <v>0.41860465116279066</v>
-      </c>
-      <c r="G14" s="39">
-        <f t="shared" ref="G14:G17" si="3">AVERAGE(B14:F14)</f>
-        <v>0.33488372093023255</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+        <f t="shared" ref="F14:F17" si="5">F3/$F$7</f>
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="G14" s="37">
+        <f t="shared" ref="G14:G17" si="6">AVERAGE(B14:F14)</f>
+        <v>0.32725534520454641</v>
+      </c>
+      <c r="K14">
+        <v>9.1218619109085644E-2</v>
+      </c>
+      <c r="L14">
+        <v>0.11985717641531594</v>
+      </c>
+      <c r="M14">
+        <v>0.1534254658385093</v>
+      </c>
+      <c r="N14">
+        <v>0.27607555125306749</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0.10179127761608781</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="12">
-        <f t="shared" si="2"/>
-        <v>0.27906976744186046</v>
+        <f t="shared" si="1"/>
+        <v>0.35714285714285715</v>
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>6.9767441860465115E-2</v>
+        <v>0.23728813559322035</v>
       </c>
       <c r="D15" s="12">
-        <f t="shared" si="2"/>
-        <v>0.13953488372093023</v>
+        <f t="shared" si="3"/>
+        <v>0.22764227642276422</v>
       </c>
       <c r="E15" s="12">
-        <f t="shared" si="2"/>
-        <v>0.41860465116279066</v>
+        <f t="shared" si="4"/>
+        <v>0.18300653594771241</v>
       </c>
       <c r="F15" s="12">
-        <f t="shared" si="2"/>
-        <v>0.41860465116279066</v>
-      </c>
-      <c r="G15" s="39">
-        <f t="shared" si="3"/>
-        <v>0.26511627906976742</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="G15" s="37">
+        <f t="shared" si="6"/>
+        <v>0.25286781287316268</v>
+      </c>
+      <c r="K15">
+        <v>0.28748276740163148</v>
+      </c>
+      <c r="L15">
+        <v>8.5913084331688983E-2</v>
+      </c>
+      <c r="M15">
+        <v>8.1605590062111794E-2</v>
+      </c>
+      <c r="N15">
+        <v>3.5495529799812076E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="36" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="12">
-        <f t="shared" si="2"/>
-        <v>9.3023255813953473E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.26785714285714285</v>
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
-        <v>4.6511627906976737E-2</v>
+        <v>0.23728813559322035</v>
       </c>
       <c r="D16" s="12">
-        <f t="shared" si="2"/>
-        <v>4.6511627906976737E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.34146341463414631</v>
       </c>
       <c r="E16" s="12">
-        <f t="shared" si="2"/>
-        <v>0.13953488372093023</v>
+        <f t="shared" si="4"/>
+        <v>0.27450980392156865</v>
       </c>
       <c r="F16" s="12">
-        <f t="shared" si="2"/>
-        <v>0.27906976744186046</v>
-      </c>
-      <c r="G16" s="39">
-        <f t="shared" si="3"/>
-        <v>0.12093023255813953</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="G16" s="37">
+        <f t="shared" si="6"/>
+        <v>0.27607555125306749</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="12">
-        <f t="shared" si="2"/>
-        <v>6.9767441860465115E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.785714285714286E-2</v>
       </c>
       <c r="C17" s="12">
         <f t="shared" si="2"/>
-        <v>4.6511627906976737E-2</v>
+        <v>5.0847457627118647E-2</v>
       </c>
       <c r="D17" s="12">
-        <f t="shared" si="2"/>
-        <v>4.6511627906976737E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.2520325203252029E-2</v>
       </c>
       <c r="E17" s="12">
-        <f t="shared" si="2"/>
-        <v>6.9767441860465115E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="F17" s="12">
-        <f t="shared" si="2"/>
-        <v>0.13953488372093023</v>
-      </c>
-      <c r="G17" s="39">
-        <f t="shared" si="3"/>
-        <v>7.441860465116279E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="G17" s="37">
+        <f t="shared" si="6"/>
+        <v>3.5495529799812076E-2</v>
+      </c>
+      <c r="K17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>8</v>
+      </c>
+      <c r="N18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>8</v>
+      </c>
+      <c r="L20">
+        <v>0.5</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>0.2</v>
+      </c>
+      <c r="M21">
+        <v>0.25</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K22" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22">
+        <f>SUM(L19:L21)</f>
+        <v>1.7</v>
+      </c>
+      <c r="M22">
+        <f t="shared" ref="M22:N22" si="7">SUM(M19:M21)</f>
+        <v>3.25</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>3</v>
+      </c>
+      <c r="M25">
+        <v>8</v>
+      </c>
+      <c r="N25">
+        <v>10</v>
+      </c>
+      <c r="O25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>3</v>
+      </c>
+      <c r="L26">
+        <f>L19/L22</f>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="M26">
+        <f>M19/$M$22</f>
+        <v>0.61538461538461542</v>
+      </c>
+      <c r="N26">
+        <f>N19/$N$22</f>
+        <v>0.5</v>
+      </c>
+      <c r="O26">
+        <f>AVERAGE(L26:N26)</f>
+        <v>0.56787330316742091</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>8</v>
+      </c>
+      <c r="L27">
+        <f>L20/L22</f>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ref="M27:M28" si="8">M20/$M$22</f>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ref="N27:N28" si="9">N20/$N$22</f>
+        <v>0.4</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ref="O27:O28" si="10">AVERAGE(L27:N27)</f>
+        <v>0.33393665158371039</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K28">
+        <v>10</v>
+      </c>
+      <c r="L28">
+        <f>L21/$L$22</f>
+        <v>0.11764705882352942</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="8"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="9"/>
+        <v>0.1</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="10"/>
+        <v>9.8190045248868804E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Load Imgae and Recipe Popup
</commit_message>
<xml_diff>
--- a/AHP Sản phẩm Món chính.xlsx
+++ b/AHP Sản phẩm Món chính.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhokk\Desktop\HoTroRaQuyetDinh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91A5AB0-4B55-4A57-A0BB-E625A9AB209D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806F43CE-777D-41B5-B550-A120B1AE48C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{738D0DCC-DACC-4475-BFCE-0371B9E87382}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="32">
   <si>
     <t>Calo</t>
   </si>
@@ -787,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8420C6-B896-437C-BDF8-F9FED97D9E93}">
-  <dimension ref="C8:AH312"/>
+  <dimension ref="C8:AH287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q266" zoomScale="57" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y282" sqref="Y282"/>
+    <sheetView tabSelected="1" topLeftCell="O262" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AB278" sqref="AB278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7917,26 +7917,26 @@
         <v>21</v>
       </c>
       <c r="V264" s="23">
-        <f t="shared" ref="V264:V272" si="65">AF66</f>
+        <f>AF66</f>
         <v>0.13012330159228624</v>
       </c>
       <c r="W264" s="23">
-        <f t="shared" ref="W264:W272" si="66">AF121</f>
+        <f t="shared" ref="W264:W272" si="65">AF121</f>
         <v>0.13936454468868514</v>
       </c>
       <c r="X264" s="23">
-        <f t="shared" ref="X264:X272" si="67">AF176</f>
+        <f t="shared" ref="X264:X272" si="66">AF176</f>
         <v>0.10818407388598128</v>
       </c>
       <c r="Y264" s="23">
-        <f t="shared" ref="Y264:Y272" si="68">AF232</f>
+        <f t="shared" ref="Y264:Y272" si="67">AF232</f>
         <v>0.20876826226802767</v>
       </c>
       <c r="AA264" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB264" s="1">
-        <v>4.7622047882677349E-2</v>
+        <v>0.36612693071609786</v>
       </c>
     </row>
     <row r="265" spans="21:34" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -7944,26 +7944,26 @@
         <v>22</v>
       </c>
       <c r="V265" s="23">
+        <f t="shared" ref="V264:V272" si="68">AF67</f>
+        <v>0.15967558329939649</v>
+      </c>
+      <c r="W265" s="23">
         <f t="shared" si="65"/>
-        <v>0.15967558329939649</v>
-      </c>
-      <c r="W265" s="23">
+        <v>0.10658520116004437</v>
+      </c>
+      <c r="X265" s="23">
         <f t="shared" si="66"/>
-        <v>0.10658520116004437</v>
-      </c>
-      <c r="X265" s="23">
+        <v>0.19112843164001372</v>
+      </c>
+      <c r="Y265" s="23">
         <f t="shared" si="67"/>
-        <v>0.19112843164001372</v>
-      </c>
-      <c r="Y265" s="23">
-        <f t="shared" si="68"/>
         <v>0.20725926507403303</v>
       </c>
       <c r="AA265" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB265" s="1">
-        <v>0.36612693071609786</v>
+        <v>0.10179127761608781</v>
       </c>
     </row>
     <row r="266" spans="21:34" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -7971,26 +7971,26 @@
         <v>23</v>
       </c>
       <c r="V266" s="23">
+        <f t="shared" si="68"/>
+        <v>0.11955493630226503</v>
+      </c>
+      <c r="W266" s="23">
         <f t="shared" si="65"/>
-        <v>0.11955493630226503</v>
-      </c>
-      <c r="W266" s="23">
+        <v>5.3364074106371985E-2</v>
+      </c>
+      <c r="X266" s="23">
         <f t="shared" si="66"/>
-        <v>5.3364074106371985E-2</v>
-      </c>
-      <c r="X266" s="23">
+        <v>6.5750307929253751E-2</v>
+      </c>
+      <c r="Y266" s="23">
         <f t="shared" si="67"/>
-        <v>6.5750307929253751E-2</v>
-      </c>
-      <c r="Y266" s="23">
-        <f t="shared" si="68"/>
         <v>0.21617473290962227</v>
       </c>
       <c r="AA266" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB266" s="1">
-        <v>0.10179127761608781</v>
+        <v>4.7622047882677349E-2</v>
       </c>
     </row>
     <row r="267" spans="21:34" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -7998,19 +7998,19 @@
         <v>24</v>
       </c>
       <c r="V267" s="23">
+        <f t="shared" si="68"/>
+        <v>0.20839562753410873</v>
+      </c>
+      <c r="W267" s="23">
         <f t="shared" si="65"/>
-        <v>0.20839562753410873</v>
-      </c>
-      <c r="W267" s="23">
+        <v>4.5520235313303327E-2</v>
+      </c>
+      <c r="X267" s="23">
         <f t="shared" si="66"/>
-        <v>4.5520235313303327E-2</v>
-      </c>
-      <c r="X267" s="23">
+        <v>3.4836738172923563E-2</v>
+      </c>
+      <c r="Y267" s="23">
         <f t="shared" si="67"/>
-        <v>3.4836738172923563E-2</v>
-      </c>
-      <c r="Y267" s="23">
-        <f t="shared" si="68"/>
         <v>1.9939826455316851E-2</v>
       </c>
     </row>
@@ -8019,19 +8019,19 @@
         <v>25</v>
       </c>
       <c r="V268" s="23">
+        <f t="shared" si="68"/>
+        <v>4.6984107440332698E-2</v>
+      </c>
+      <c r="W268" s="23">
         <f t="shared" si="65"/>
-        <v>4.6984107440332698E-2</v>
-      </c>
-      <c r="W268" s="23">
+        <v>4.1672704890969761E-2</v>
+      </c>
+      <c r="X268" s="23">
         <f t="shared" si="66"/>
-        <v>4.1672704890969761E-2</v>
-      </c>
-      <c r="X268" s="23">
+        <v>6.0950894117200262E-2</v>
+      </c>
+      <c r="Y268" s="23">
         <f t="shared" si="67"/>
-        <v>6.0950894117200262E-2</v>
-      </c>
-      <c r="Y268" s="23">
-        <f t="shared" si="68"/>
         <v>3.3337175407322867E-2</v>
       </c>
     </row>
@@ -8040,19 +8040,19 @@
         <v>26</v>
       </c>
       <c r="V269" s="23">
+        <f t="shared" si="68"/>
+        <v>3.3961417599796546E-2</v>
+      </c>
+      <c r="W269" s="23">
         <f t="shared" si="65"/>
-        <v>3.3961417599796546E-2</v>
-      </c>
-      <c r="W269" s="23">
+        <v>0.21725170556913689</v>
+      </c>
+      <c r="X269" s="23">
         <f t="shared" si="66"/>
-        <v>0.21725170556913689</v>
-      </c>
-      <c r="X269" s="23">
+        <v>0.17540835050411108</v>
+      </c>
+      <c r="Y269" s="23">
         <f t="shared" si="67"/>
-        <v>0.17540835050411108</v>
-      </c>
-      <c r="Y269" s="23">
-        <f t="shared" si="68"/>
         <v>3.9652153375599929E-2</v>
       </c>
     </row>
@@ -8061,19 +8061,19 @@
         <v>27</v>
       </c>
       <c r="V270" s="23">
+        <f t="shared" si="68"/>
+        <v>3.3448769813035725E-2</v>
+      </c>
+      <c r="W270" s="23">
         <f t="shared" si="65"/>
-        <v>3.3448769813035725E-2</v>
-      </c>
-      <c r="W270" s="23">
+        <v>0.16515664303048702</v>
+      </c>
+      <c r="X270" s="23">
         <f t="shared" si="66"/>
-        <v>0.16515664303048702</v>
-      </c>
-      <c r="X270" s="23">
+        <v>0.10010674337750672</v>
+      </c>
+      <c r="Y270" s="23">
         <f t="shared" si="67"/>
-        <v>0.10010674337750672</v>
-      </c>
-      <c r="Y270" s="23">
-        <f t="shared" si="68"/>
         <v>4.2899733609935133E-2</v>
       </c>
     </row>
@@ -8082,19 +8082,19 @@
         <v>28</v>
       </c>
       <c r="V271" s="23">
+        <f t="shared" si="68"/>
+        <v>2.0100612443774143E-2</v>
+      </c>
+      <c r="W271" s="23">
         <f t="shared" si="65"/>
-        <v>2.0100612443774143E-2</v>
-      </c>
-      <c r="W271" s="23">
+        <v>0.11258799542525699</v>
+      </c>
+      <c r="X271" s="23">
         <f t="shared" si="66"/>
-        <v>0.11258799542525699</v>
-      </c>
-      <c r="X271" s="23">
+        <v>6.3778538577927701E-2</v>
+      </c>
+      <c r="Y271" s="23">
         <f t="shared" si="67"/>
-        <v>6.3778538577927701E-2</v>
-      </c>
-      <c r="Y271" s="23">
-        <f t="shared" si="68"/>
         <v>8.2235119558031783E-2</v>
       </c>
     </row>
@@ -8103,19 +8103,19 @@
         <v>29</v>
       </c>
       <c r="V272" s="23">
+        <f t="shared" si="68"/>
+        <v>1.9087052872023651E-2</v>
+      </c>
+      <c r="W272" s="23">
         <f t="shared" si="65"/>
-        <v>1.9087052872023651E-2</v>
-      </c>
-      <c r="W272" s="23">
+        <v>5.6193397786274801E-2</v>
+      </c>
+      <c r="X272" s="23">
         <f t="shared" si="66"/>
-        <v>5.6193397786274801E-2</v>
-      </c>
-      <c r="X272" s="23">
+        <v>0.16183368987062691</v>
+      </c>
+      <c r="Y272" s="23">
         <f t="shared" si="67"/>
-        <v>0.16183368987062691</v>
-      </c>
-      <c r="Y272" s="23">
-        <f t="shared" si="68"/>
         <v>5.6967661963612561E-2</v>
       </c>
     </row>
@@ -8136,7 +8136,7 @@
       </c>
       <c r="V278" s="23">
         <f>MMULT(V263:Y263,AB263:AB266)</f>
-        <v>0.13711148701881229</v>
+        <v>0.14187975732710059</v>
       </c>
       <c r="W278" s="26">
         <f>RANK(V278,V278:V287,0)</f>
@@ -8149,7 +8149,7 @@
       </c>
       <c r="V279" s="23">
         <f>MMULT(V264:Y264,AB263:AB266)</f>
-        <v>0.13053621743637811</v>
+        <v>0.13501878162806846</v>
       </c>
       <c r="W279" s="26">
         <f>RANK(V279,V278:V287,0)</f>
@@ -8162,7 +8162,7 @@
       </c>
       <c r="V280" s="23">
         <f>MMULT(V265:Y265,AB263:AB266)</f>
-        <v>0.17350664916579334</v>
+        <v>0.14570542262533306</v>
       </c>
       <c r="W280" s="26">
         <f>RANK(V280,V278:V287,0)</f>
@@ -8175,11 +8175,11 @@
       </c>
       <c r="V281" s="23">
         <f>MMULT(V266:Y266,AB263:AB266)</f>
-        <v>0.10653852098851505</v>
+        <v>9.4445069801732992E-2</v>
       </c>
       <c r="W281" s="26">
         <f>RANK(V281,V278:V287,0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="282" spans="21:23" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -8188,7 +8188,7 @@
       </c>
       <c r="V282" s="23">
         <f>MMULT(V267:Y267,AB263:AB266)</f>
-        <v>0.11791142758058061</v>
+        <v>0.12212112781867783</v>
       </c>
       <c r="W282" s="26">
         <f>RANK(V282,V278:V287,0)</f>
@@ -8201,11 +8201,11 @@
       </c>
       <c r="V283" s="23">
         <f>MMULT(V268:Y268,AB263:AB266)</f>
-        <v>5.0455645664590779E-2</v>
+        <v>4.5811262136438852E-2</v>
       </c>
       <c r="W283" s="26">
         <f>RANK(V283,V278:V287,0)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="284" spans="21:23" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -8214,11 +8214,11 @@
       </c>
       <c r="V284" s="23">
         <f>MMULT(V269:Y269,AB263:AB266)</f>
-        <v>9.5056875138559288E-2</v>
+        <v>0.11573799667089105</v>
       </c>
       <c r="W284" s="26">
         <f>RANK(V284,V278:V287,0)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="285" spans="21:23" ht="21" x14ac:dyDescent="0.3">
@@ -8227,11 +8227,11 @@
       </c>
       <c r="V285" s="23">
         <f>MMULT(V270:Y270,AB263:AB266)</f>
-        <v>6.5088273406427116E-2</v>
+        <v>8.8905843728186426E-2</v>
       </c>
       <c r="W285" s="26">
         <f>RANK(V285,V278:V287,0)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="286" spans="21:23" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -8240,11 +8240,11 @@
       </c>
       <c r="V286" s="23">
         <f>MMULT(V271:Y271,AB263:AB266)</f>
-        <v>4.6821466923410091E-2</v>
+        <v>6.1367738482527051E-2</v>
       </c>
       <c r="W286" s="26">
         <f>RANK(V286,V278:V287,0)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="287" spans="21:23" ht="21" x14ac:dyDescent="0.3">
@@ -8253,205 +8253,11 @@
       </c>
       <c r="V287" s="23">
         <f>MMULT(V272:Y272,AB263:AB266)</f>
-        <v>7.697343667693328E-2</v>
+        <v>4.9006999781043684E-2</v>
       </c>
       <c r="W287" s="26">
         <f>RANK(V287,V278:V287,0)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="299" spans="21:28" ht="21" x14ac:dyDescent="0.3">
-      <c r="U299" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="V299" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="W299" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="X299" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y299" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA299" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB299" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="300" spans="21:28" ht="21" x14ac:dyDescent="0.3">
-      <c r="U300" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="V300" s="23">
-        <f>AF102</f>
-        <v>0</v>
-      </c>
-      <c r="W300" s="23">
-        <f>AF157</f>
-        <v>0</v>
-      </c>
-      <c r="X300" s="23">
-        <f>AF212</f>
-        <v>0</v>
-      </c>
-      <c r="Y300" s="23">
-        <f>AF268</f>
-        <v>0</v>
-      </c>
-      <c r="AA300" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB300" s="1">
-        <v>0.48445974378513695</v>
-      </c>
-    </row>
-    <row r="301" spans="21:28" ht="21" x14ac:dyDescent="0.3">
-      <c r="U301" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="V301" s="23">
-        <f t="shared" ref="V301:V303" si="69">AF103</f>
-        <v>0</v>
-      </c>
-      <c r="W301" s="23">
-        <f t="shared" ref="W301:W303" si="70">AF158</f>
-        <v>0</v>
-      </c>
-      <c r="X301" s="23">
-        <f t="shared" ref="X301:X303" si="71">AF213</f>
-        <v>0</v>
-      </c>
-      <c r="Y301" s="23">
-        <f t="shared" ref="Y301:Y303" si="72">AF269</f>
-        <v>0</v>
-      </c>
-      <c r="AA301" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB301" s="1">
-        <v>4.7622047882677349E-2</v>
-      </c>
-    </row>
-    <row r="302" spans="21:28" ht="21" x14ac:dyDescent="0.3">
-      <c r="U302" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="V302" s="23">
-        <f t="shared" si="69"/>
-        <v>0</v>
-      </c>
-      <c r="W302" s="23">
-        <f t="shared" si="70"/>
-        <v>0</v>
-      </c>
-      <c r="X302" s="23">
-        <f t="shared" si="71"/>
-        <v>0</v>
-      </c>
-      <c r="Y302" s="23">
-        <f t="shared" si="72"/>
-        <v>0</v>
-      </c>
-      <c r="AA302" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB302" s="1">
-        <v>0.36612693071609786</v>
-      </c>
-    </row>
-    <row r="303" spans="21:28" ht="21" x14ac:dyDescent="0.3">
-      <c r="U303" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="V303" s="23">
-        <f t="shared" si="69"/>
-        <v>0</v>
-      </c>
-      <c r="W303" s="23">
-        <f t="shared" si="70"/>
-        <v>0</v>
-      </c>
-      <c r="X303" s="23">
-        <f t="shared" si="71"/>
-        <v>0</v>
-      </c>
-      <c r="Y303" s="23">
-        <f t="shared" si="72"/>
-        <v>0</v>
-      </c>
-      <c r="AA303" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB303" s="1">
-        <v>0.10179127761608781</v>
-      </c>
-    </row>
-    <row r="308" spans="21:23" ht="21" x14ac:dyDescent="0.3">
-      <c r="U308" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="V308" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="W308" s="25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="309" spans="21:23" ht="21" x14ac:dyDescent="0.3">
-      <c r="U309" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="V309" s="23" t="e">
-        <f>MMULT(V294:Y294,AB294:AB297)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="W309" s="26" t="e">
-        <f>RANK(V309,V309:V318,0)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="310" spans="21:23" ht="21" x14ac:dyDescent="0.3">
-      <c r="U310" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="V310" s="23" t="e">
-        <f>MMULT(V295:Y295,AB294:AB297)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="W310" s="26" t="e">
-        <f>RANK(V310,V309:V318,0)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="311" spans="21:23" ht="21" x14ac:dyDescent="0.3">
-      <c r="U311" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="V311" s="23" t="e">
-        <f>MMULT(V296:Y296,AB294:AB297)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="W311" s="26" t="e">
-        <f>RANK(V311,V309:V318,0)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="312" spans="21:23" ht="21" x14ac:dyDescent="0.3">
-      <c r="U312" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="V312" s="23" t="e">
-        <f>MMULT(V297:Y297,AB294:AB297)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="W312" s="26" t="e">
-        <f>RANK(V312,V309:V318,0)</f>
-        <v>#VALUE!</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -8489,8 +8295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E685A3B-2712-4D4E-B3A3-A2F89ADEC8D7}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8527,10 +8333,10 @@
       </c>
       <c r="P1">
         <f>MMULT(K11:N11,R11:R14)</f>
-        <v>0.21732096108564508</v>
+        <v>0.23315710002512757</v>
       </c>
       <c r="Q1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="108" x14ac:dyDescent="0.3">
@@ -8547,20 +8353,20 @@
         <v>0.25</v>
       </c>
       <c r="E2" s="12">
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="F2" s="12">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="O2" s="27" t="s">
         <v>21</v>
       </c>
       <c r="P2">
         <f>MMULT(K12:N12,R11:R14)</f>
-        <v>0.19748300480093944</v>
+        <v>0.23330288921802478</v>
       </c>
       <c r="Q2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="72" x14ac:dyDescent="0.3">
@@ -8574,20 +8380,20 @@
         <v>1</v>
       </c>
       <c r="D3" s="12">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E3" s="12">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F3" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O3" s="27" t="s">
         <v>22</v>
       </c>
       <c r="P3">
         <f>MMULT(K13:N13,R11:R14)</f>
-        <v>0.27416483869477615</v>
+        <v>0.23597463567649724</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -8601,23 +8407,23 @@
         <v>4</v>
       </c>
       <c r="C4" s="12">
-        <v>0.66666666666666663</v>
+        <v>2</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
       </c>
       <c r="E4" s="12">
-        <v>0.66666666666666663</v>
+        <v>3</v>
       </c>
       <c r="F4" s="12">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O4" s="27" t="s">
         <v>23</v>
       </c>
       <c r="P4">
         <f>MMULT(K14:N14,R11:R14)</f>
-        <v>0.13417487101811071</v>
+        <v>0.11683934627481456</v>
       </c>
       <c r="Q4">
         <v>5</v>
@@ -8628,26 +8434,26 @@
         <v>23</v>
       </c>
       <c r="B5" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="12">
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="D5" s="12">
-        <v>1.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E5" s="12">
         <v>1</v>
       </c>
       <c r="F5" s="12">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O5" s="27" t="s">
         <v>24</v>
       </c>
       <c r="P5">
         <f>MMULT(K15:N15,R11:R14)</f>
-        <v>0.17685632440052859</v>
+        <v>0.18072602880553582</v>
       </c>
       <c r="Q5">
         <v>4</v>
@@ -8658,16 +8464,16 @@
         <v>24</v>
       </c>
       <c r="B6" s="12">
-        <v>0.2</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C6" s="12">
-        <v>0.14285714285714285</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D6" s="12">
-        <v>0.14285714285714285</v>
+        <v>0.25</v>
       </c>
       <c r="E6" s="12">
-        <v>0.14285714285714285</v>
+        <v>0.5</v>
       </c>
       <c r="F6" s="12">
         <v>1</v>
@@ -8679,23 +8485,23 @@
       </c>
       <c r="B7" s="36">
         <f>SUM(B2:B6)</f>
-        <v>11.2</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="C7" s="36">
         <f t="shared" ref="C7:F7" si="0">SUM(C2:C6)</f>
-        <v>2.8095238095238093</v>
+        <v>4.1666666666666661</v>
       </c>
       <c r="D7" s="36">
         <f t="shared" si="0"/>
-        <v>4.3928571428571432</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="E7" s="36">
         <f t="shared" si="0"/>
-        <v>3.6428571428571428</v>
+        <v>7</v>
       </c>
       <c r="F7" s="36">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -8761,7 +8567,7 @@
         <v>0.32725534520454641</v>
       </c>
       <c r="R12" s="1">
-        <v>4.7622047882677349E-2</v>
+        <v>0.36612693071609786</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="36" x14ac:dyDescent="0.3">
@@ -8770,27 +8576,27 @@
       </c>
       <c r="B13" s="38">
         <f>B2/$B$7</f>
-        <v>8.9285714285714288E-2</v>
+        <v>9.375E-2</v>
       </c>
       <c r="C13" s="12">
         <f>C2/$C$7</f>
-        <v>0.11864406779661017</v>
+        <v>0.08</v>
       </c>
       <c r="D13" s="12">
         <f>D2/$D$7</f>
-        <v>5.6910569105691054E-2</v>
+        <v>0.10714285714285714</v>
       </c>
       <c r="E13" s="12">
         <f>E2/$E$7</f>
-        <v>9.1503267973856203E-2</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="F13" s="12">
         <f>F2/$F$7</f>
-        <v>0.18518518518518517</v>
+        <v>0.13043478260869565</v>
       </c>
       <c r="G13" s="37">
         <f>AVERAGE(B13:F13)</f>
-        <v>0.10830576086941139</v>
+        <v>9.6551242236024848E-2</v>
       </c>
       <c r="K13">
         <v>0.1753747266931851</v>
@@ -8805,7 +8611,7 @@
         <v>0.25286781287316268</v>
       </c>
       <c r="R13" s="1">
-        <v>0.36612693071609786</v>
+        <v>0.10179127761608781</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="36" x14ac:dyDescent="0.3">
@@ -8813,28 +8619,28 @@
         <v>21</v>
       </c>
       <c r="B14" s="12">
-        <f t="shared" ref="B14:F17" si="1">B3/$B$7</f>
-        <v>0.26785714285714285</v>
+        <f t="shared" ref="B14:B17" si="1">B3/$B$7</f>
+        <v>0.28125</v>
       </c>
       <c r="C14" s="12">
         <f t="shared" ref="C14:C17" si="2">C3/$C$7</f>
-        <v>0.35593220338983056</v>
+        <v>0.24000000000000005</v>
       </c>
       <c r="D14" s="12">
         <f t="shared" ref="D14:D17" si="3">D3/$D$7</f>
-        <v>0.34146341463414631</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="E14" s="12">
         <f t="shared" ref="E14:E17" si="4">E3/$E$7</f>
-        <v>0.41176470588235292</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="F14" s="12">
         <f t="shared" ref="F14:F17" si="5">F3/$F$7</f>
-        <v>0.25925925925925924</v>
+        <v>0.2608695652173913</v>
       </c>
       <c r="G14" s="37">
         <f t="shared" ref="G14:G17" si="6">AVERAGE(B14:F14)</f>
-        <v>0.32725534520454641</v>
+        <v>0.25642391304347828</v>
       </c>
       <c r="K14">
         <v>9.1218619109085644E-2</v>
@@ -8849,7 +8655,7 @@
         <v>0.27607555125306749</v>
       </c>
       <c r="R14" s="1">
-        <v>0.10179127761608781</v>
+        <v>4.7622047882677349E-2</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.3">
@@ -8858,27 +8664,27 @@
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
-        <v>0.35714285714285715</v>
+        <v>0.375</v>
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>0.23728813559322035</v>
+        <v>0.48000000000000009</v>
       </c>
       <c r="D15" s="12">
         <f t="shared" si="3"/>
-        <v>0.22764227642276422</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="E15" s="12">
         <f t="shared" si="4"/>
-        <v>0.18300653594771241</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="F15" s="12">
         <f t="shared" si="5"/>
-        <v>0.25925925925925924</v>
+        <v>0.34782608695652173</v>
       </c>
       <c r="G15" s="37">
         <f t="shared" si="6"/>
-        <v>0.25286781287316268</v>
+        <v>0.41199378881987575</v>
       </c>
       <c r="K15">
         <v>0.28748276740163148</v>
@@ -8899,27 +8705,27 @@
       </c>
       <c r="B16" s="12">
         <f t="shared" si="1"/>
-        <v>0.26785714285714285</v>
+        <v>0.1875</v>
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
-        <v>0.23728813559322035</v>
+        <v>0.12000000000000002</v>
       </c>
       <c r="D16" s="12">
         <f t="shared" si="3"/>
-        <v>0.34146341463414631</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="E16" s="12">
         <f t="shared" si="4"/>
-        <v>0.27450980392156865</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="F16" s="12">
         <f t="shared" si="5"/>
-        <v>0.25925925925925924</v>
+        <v>0.17391304347826086</v>
       </c>
       <c r="G16" s="37">
         <f t="shared" si="6"/>
-        <v>0.27607555125306749</v>
+        <v>0.1534254658385093</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="36" x14ac:dyDescent="0.3">
@@ -8928,27 +8734,27 @@
       </c>
       <c r="B17" s="12">
         <f t="shared" si="1"/>
-        <v>1.785714285714286E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C17" s="12">
         <f t="shared" si="2"/>
-        <v>5.0847457627118647E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D17" s="12">
         <f t="shared" si="3"/>
-        <v>3.2520325203252029E-2</v>
+        <v>0.10714285714285714</v>
       </c>
       <c r="E17" s="12">
         <f t="shared" si="4"/>
-        <v>3.9215686274509803E-2</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="F17" s="12">
         <f t="shared" si="5"/>
-        <v>3.7037037037037035E-2</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="G17" s="37">
         <f t="shared" si="6"/>
-        <v>3.5495529799812076E-2</v>
+        <v>8.1605590062111794E-2</v>
       </c>
       <c r="K17" t="s">
         <v>3</v>

</xml_diff>